<commit_message>
feat: update ps music
修改ps背景音乐
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Music_音效表.xlsx
+++ b/pet-simulator/Excel/Music_音效表.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\pet-simulator\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785A849A-5359-49E2-AEE6-98EB03AC8E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="16384" windowHeight="8192" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,46 +136,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="36">
-    <numFmt numFmtId="176" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="177" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="179" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="184" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="185" formatCode="yy/m/d"/>
-    <numFmt numFmtId="186" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="187" formatCode="mmmmm"/>
-    <numFmt numFmtId="188" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="189" formatCode="m/d"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="190" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="191" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="192" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="193" formatCode="#\ ??"/>
-    <numFmt numFmtId="194" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="195" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="196" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="197" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="198" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="199" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -184,163 +151,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,194 +175,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -554,241 +184,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -815,61 +213,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1127,36 +481,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALT19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D$1:D$1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="9" style="4"/>
-    <col min="3" max="3" width="75.9666666666667" style="4" customWidth="1"/>
+    <col min="3" max="3" width="76" style="4" customWidth="1"/>
     <col min="4" max="5" width="9" style="4"/>
     <col min="6" max="6" width="12.875" style="4" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="19.375" style="4" customWidth="1"/>
     <col min="9" max="9" width="21.75" style="4" customWidth="1"/>
     <col min="10" max="980" width="9" style="4"/>
-    <col min="981" max="987" width="11.6416666666667" style="4" customWidth="1"/>
+    <col min="981" max="987" width="11.625" style="4" customWidth="1"/>
     <col min="988" max="988" width="9" style="4"/>
-    <col min="989" max="999" width="11.6416666666667" style="4" customWidth="1"/>
+    <col min="989" max="999" width="11.625" style="4" customWidth="1"/>
     <col min="1000" max="1008" width="9" style="4"/>
-    <col min="1009" max="1022" width="11.6416666666667" customWidth="1"/>
+    <col min="1009" max="1022" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:9">
+    <row r="1" spans="1:1008" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:9">
+    <row r="2" spans="1:1008" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:9">
+    <row r="3" spans="1:1008" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1243,7 +597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:1008">
+    <row r="5" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -1254,7 +608,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2261,7 +1615,7 @@
       <c r="ALS5" s="5"/>
       <c r="ALT5" s="5"/>
     </row>
-    <row r="6" s="2" customFormat="1" ht="17.1" customHeight="1" spans="1:1008">
+    <row r="6" spans="1:1008" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -3279,7 +2633,7 @@
       <c r="ALS6" s="5"/>
       <c r="ALT6" s="5"/>
     </row>
-    <row r="7" s="2" customFormat="1" ht="17.1" customHeight="1" spans="1:1008">
+    <row r="7" spans="1:1008" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -4297,7 +3651,7 @@
       <c r="ALS7" s="5"/>
       <c r="ALT7" s="5"/>
     </row>
-    <row r="8" s="2" customFormat="1" spans="1:1008">
+    <row r="8" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -5315,7 +4669,7 @@
       <c r="ALS8" s="5"/>
       <c r="ALT8" s="5"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:1008" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -5329,7 +4683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:1008" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -5343,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="1" spans="1:1008">
+    <row r="11" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -6361,7 +5715,7 @@
       <c r="ALS11" s="5"/>
       <c r="ALT11" s="5"/>
     </row>
-    <row r="12" s="2" customFormat="1" spans="1:1008">
+    <row r="12" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -7379,7 +6733,7 @@
       <c r="ALS12" s="5"/>
       <c r="ALT12" s="5"/>
     </row>
-    <row r="13" s="3" customFormat="1" spans="1:1008">
+    <row r="13" spans="1:1008" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -8397,7 +7751,7 @@
       <c r="ALS13" s="6"/>
       <c r="ALT13" s="6"/>
     </row>
-    <row r="14" s="2" customFormat="1" spans="1:1008">
+    <row r="14" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -9415,7 +8769,7 @@
       <c r="ALS14" s="5"/>
       <c r="ALT14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:1008" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -9435,7 +8789,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" spans="1:1008">
+    <row r="16" spans="1:1008" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -10453,7 +9807,7 @@
       <c r="ALS16" s="5"/>
       <c r="ALT16" s="5"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:1008" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -10467,7 +9821,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:1008" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -10481,7 +9835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="1" spans="1:1008">
+    <row r="19" spans="1:1008" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6">
         <v>15</v>
       </c>
@@ -11501,13 +10855,20 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+</pixelators>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
     <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0">
@@ -11520,15 +10881,8 @@
 </woProps>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-</pixelators>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -11537,7 +10891,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>

</xml_diff>